<commit_message>
Adding econ project stuff
</commit_message>
<xml_diff>
--- a/1_Planning/Receipts/Receipts.xlsx
+++ b/1_Planning/Receipts/Receipts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Receipt</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Removed cost of personal items (magnets)</t>
+  </si>
+  <si>
+    <t>2018-04-10_3D_Hubs_High_Speed_Prototype.pdf</t>
+  </si>
+  <si>
+    <t>High speed prototype 3D printing</t>
+  </si>
+  <si>
+    <t>X-Axis high speed motor, more belt, more pulley</t>
   </si>
 </sst>
 </file>
@@ -165,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +197,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,17 +227,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -499,7 +524,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,8 +751,8 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -777,10 +802,30 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2">
+        <v>75.33</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="2"/>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
@@ -800,7 +845,7 @@
       </c>
       <c r="D31" s="3">
         <f>SUM(D2:D30)</f>
-        <v>835.82</v>
+        <v>911.15000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schematics and layout
</commit_message>
<xml_diff>
--- a/1_Planning/Receipts/Receipts.xlsx
+++ b/1_Planning/Receipts/Receipts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Receipt</t>
   </si>
@@ -158,13 +158,25 @@
     <t>Removed cost of personal items (magnets)</t>
   </si>
   <si>
-    <t>2018-04-10_3D_Hubs_High_Speed_Prototype.pdf</t>
-  </si>
-  <si>
-    <t>High speed prototype 3D printing</t>
-  </si>
-  <si>
     <t>X-Axis high speed motor, more belt, more pulley</t>
+  </si>
+  <si>
+    <t>2018-06-07_Bearings_Canada.pdf</t>
+  </si>
+  <si>
+    <t>1/2" Linear bearings for high speed system</t>
+  </si>
+  <si>
+    <t>2018-06-07_Metal_Supermarkets.pdf</t>
+  </si>
+  <si>
+    <t>1/2" Linear rods for high speed system</t>
+  </si>
+  <si>
+    <t>2018-06-07_3D_Hubs.pdf</t>
+  </si>
+  <si>
+    <t>High speed system mounting brackets</t>
   </si>
 </sst>
 </file>
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,50 +814,66 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2">
-        <v>75.33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5" t="s">
-        <v>41</v>
+      <c r="D20" s="2">
+        <v>99.99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>40.909999999999997</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C31" s="1" t="s">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2">
+        <v>72.150000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="3">
-        <f>SUM(D2:D30)</f>
-        <v>911.15000000000009</v>
+      <c r="D29" s="3">
+        <f>SUM(D2:D28)</f>
+        <v>1048.8700000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>